<commit_message>
Tudo terminado, menos os DS
Alteração em tudo praticamente. Nunca mais vou mexer com essa parte da documentação.

Agora só falta terminar os diagramas de sequência, transformar eles em PNG e colocar todos os diagramas atualizados e novos no documento do TCC.

Tá quase acabando.
</commit_message>
<xml_diff>
--- a/Banco de dados/Dicionário de Dados/Dicionário de Dados - Samaforte.xlsx
+++ b/Banco de dados/Dicionário de Dados/Dicionário de Dados - Samaforte.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="165">
   <si>
     <t>Tabela</t>
   </si>
@@ -298,6 +298,9 @@
     <t>UQ</t>
   </si>
   <si>
+    <t>CPF do cliente.</t>
+  </si>
+  <si>
     <t>endereco</t>
   </si>
   <si>
@@ -327,6 +330,21 @@
     <t>Valor da venda.</t>
   </si>
   <si>
+    <t>desconto</t>
+  </si>
+  <si>
+    <t>Desconto sobre o valor da venda.</t>
+  </si>
+  <si>
+    <t>forma_pagamento</t>
+  </si>
+  <si>
+    <t>VARCHAR(45)</t>
+  </si>
+  <si>
+    <t>Forma de pagamento.</t>
+  </si>
+  <si>
     <t>id_usuario</t>
   </si>
   <si>
@@ -343,25 +361,48 @@
     <t>Id do orçamento ligado a venda.</t>
   </si>
   <si>
+    <t>Código de identificação
+ do orçamento.</t>
+  </si>
+  <si>
     <t>dataCriacao</t>
   </si>
   <si>
     <t>DATATIME</t>
   </si>
   <si>
+    <t>Data de criação do orçamento.</t>
+  </si>
+  <si>
     <t>dataValidade</t>
   </si>
   <si>
+    <t>Data de validade do orçamento.</t>
+  </si>
+  <si>
     <t>VARCHAR(20)</t>
   </si>
   <si>
+    <t>"pendente"</t>
+  </si>
+  <si>
+    <t>Status de venda do orçamento.</t>
+  </si>
+  <si>
     <t>informacoes</t>
   </si>
   <si>
     <t>TEXT</t>
   </si>
   <si>
+    <t>Informações adicionais que o ator 
+queira colocar no orçamento.</t>
+  </si>
+  <si>
     <t>id_cliente</t>
+  </si>
+  <si>
+    <t>Id do cliente ligado ao orçamento.</t>
   </si>
   <si>
     <t>Código de identificação
@@ -1216,7 +1257,7 @@
         <v>47</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>132</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4">
@@ -1234,7 +1275,7 @@
         <v>47</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>133</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5">
@@ -1252,16 +1293,16 @@
         <v>47</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>134</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" s="7"/>
       <c r="C6" s="3" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>79</v>
@@ -1270,13 +1311,13 @@
         <v>47</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>135</v>
+        <v>148</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="7"/>
       <c r="C7" s="2" t="s">
-        <v>136</v>
+        <v>149</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>50</v>
@@ -1288,13 +1329,13 @@
         <v>47</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>137</v>
+        <v>150</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" s="5"/>
       <c r="C8" s="3" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>45</v>
@@ -1306,7 +1347,7 @@
         <v>47</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>138</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -1375,13 +1416,13 @@
         <v>47</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>139</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" s="7"/>
       <c r="C4" s="3" t="s">
-        <v>140</v>
+        <v>153</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>45</v>
@@ -1399,7 +1440,7 @@
     <row r="5">
       <c r="B5" s="5"/>
       <c r="C5" s="2" t="s">
-        <v>141</v>
+        <v>154</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>45</v>
@@ -1480,13 +1521,13 @@
         <v>47</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>142</v>
+        <v>155</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" s="7"/>
       <c r="C4" s="3" t="s">
-        <v>143</v>
+        <v>156</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>45</v>
@@ -1498,13 +1539,13 @@
         <v>47</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>144</v>
+        <v>157</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" s="7"/>
       <c r="C5" s="2" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>45</v>
@@ -1516,7 +1557,7 @@
         <v>47</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>145</v>
+        <v>158</v>
       </c>
     </row>
     <row r="6">
@@ -1534,7 +1575,7 @@
         <v>47</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>146</v>
+        <v>159</v>
       </c>
     </row>
     <row r="7">
@@ -1552,16 +1593,16 @@
         <v>47</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>147</v>
+        <v>160</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" s="7"/>
       <c r="C8" s="9" t="s">
-        <v>148</v>
+        <v>161</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E8" s="9" t="s">
         <v>79</v>
@@ -1570,16 +1611,16 @@
         <v>47</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>149</v>
+        <v>162</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" s="5"/>
       <c r="C9" s="2" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>54</v>
@@ -1588,7 +1629,7 @@
         <v>47</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>151</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -2079,13 +2120,13 @@
         <v>47</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>58</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="5"/>
       <c r="C7" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>50</v>
@@ -2097,7 +2138,7 @@
         <v>47</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -2166,16 +2207,16 @@
         <v>47</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" s="7"/>
       <c r="C4" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>79</v>
@@ -2184,66 +2225,102 @@
         <v>47</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" s="7"/>
       <c r="C5" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>66</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>47</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" s="7"/>
-      <c r="C6" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="E6" s="3" t="s">
+      <c r="C6" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="F6" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="G6" s="3" t="s">
+      <c r="D6" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="F6" s="9">
+        <v>0.0</v>
+      </c>
+      <c r="G6" s="9" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="7">
-      <c r="B7" s="5"/>
+      <c r="B7" s="7"/>
       <c r="C7" s="2" t="s">
         <v>96</v>
       </c>
       <c r="D7" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" s="7"/>
+      <c r="C8" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>97</v>
+      <c r="E8" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" s="5"/>
+      <c r="C9" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B3:B7"/>
+    <mergeCell ref="B3:B9"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins bottom="1.0" footer="0.0" header="0.0" left="1.0" right="1.0" top="1.0"/>
@@ -2307,16 +2384,16 @@
         <v>47</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>48</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" s="7"/>
       <c r="C4" s="3" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>54</v>
@@ -2325,16 +2402,16 @@
         <v>47</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>51</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" s="7"/>
       <c r="C5" s="2" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>54</v>
@@ -2343,7 +2420,7 @@
         <v>47</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>55</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6">
@@ -2352,40 +2429,40 @@
         <v>71</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>54</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>47</v>
+        <v>111</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>58</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="7"/>
       <c r="C7" s="2" t="s">
-        <v>102</v>
+        <v>113</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>103</v>
+        <v>114</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>47</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>60</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" s="5"/>
       <c r="C8" s="3" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>45</v>
@@ -2397,7 +2474,7 @@
         <v>47</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>62</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -2466,7 +2543,7 @@
         <v>47</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>105</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4">
@@ -2484,7 +2561,7 @@
         <v>47</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>106</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5">
@@ -2502,16 +2579,16 @@
         <v>47</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>107</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" s="7"/>
       <c r="C6" s="3" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>109</v>
+        <v>122</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>79</v>
@@ -2520,13 +2597,13 @@
         <v>47</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="7"/>
       <c r="C7" s="2" t="s">
-        <v>111</v>
+        <v>124</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>50</v>
@@ -2538,7 +2615,7 @@
         <v>47</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>112</v>
+        <v>125</v>
       </c>
     </row>
     <row r="8">
@@ -2556,13 +2633,13 @@
         <v>47</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>113</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" s="7"/>
       <c r="C9" s="2" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>53</v>
@@ -2574,13 +2651,13 @@
         <v>47</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>115</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" s="7"/>
       <c r="C10" s="3" t="s">
-        <v>116</v>
+        <v>129</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>45</v>
@@ -2592,7 +2669,7 @@
         <v>47</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>117</v>
+        <v>130</v>
       </c>
     </row>
     <row r="11">
@@ -2610,7 +2687,7 @@
         <v>1.0</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>118</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -2679,7 +2756,7 @@
         <v>47</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>119</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4">
@@ -2688,7 +2765,7 @@
         <v>52</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>120</v>
+        <v>133</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>54</v>
@@ -2697,13 +2774,13 @@
         <v>47</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>121</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" s="7"/>
       <c r="C5" s="2" t="s">
-        <v>122</v>
+        <v>135</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>50</v>
@@ -2715,7 +2792,7 @@
         <v>47</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>123</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6">
@@ -2733,7 +2810,7 @@
         <v>47</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>124</v>
+        <v>137</v>
       </c>
     </row>
     <row r="7">
@@ -2751,7 +2828,7 @@
         <v>1.0</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>125</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -2820,7 +2897,7 @@
         <v>47</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>126</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4">
@@ -2829,7 +2906,7 @@
         <v>52</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>120</v>
+        <v>133</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>79</v>
@@ -2838,7 +2915,7 @@
         <v>47</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>127</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5">
@@ -2856,13 +2933,13 @@
         <v>47</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>128</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" s="7"/>
       <c r="C6" s="3" t="s">
-        <v>129</v>
+        <v>142</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>72</v>
@@ -2874,7 +2951,7 @@
         <v>47</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>130</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7">
@@ -2892,7 +2969,7 @@
         <v>1.0</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>131</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Docs diagrama sequencia (#11)
* Tudo terminado, menos os DS

Alteração em tudo praticamente. Nunca mais vou mexer com essa parte da documentação.

Agora só falta terminar os diagramas de sequência, transformar eles em PNG e colocar todos os diagramas atualizados e novos no documento do TCC.

Tá quase acabando.

* D.S finalizados
</commit_message>
<xml_diff>
--- a/Banco de dados/Dicionário de Dados/Dicionário de Dados - Samaforte.xlsx
+++ b/Banco de dados/Dicionário de Dados/Dicionário de Dados - Samaforte.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="165">
   <si>
     <t>Tabela</t>
   </si>
@@ -298,6 +298,9 @@
     <t>UQ</t>
   </si>
   <si>
+    <t>CPF do cliente.</t>
+  </si>
+  <si>
     <t>endereco</t>
   </si>
   <si>
@@ -327,6 +330,21 @@
     <t>Valor da venda.</t>
   </si>
   <si>
+    <t>desconto</t>
+  </si>
+  <si>
+    <t>Desconto sobre o valor da venda.</t>
+  </si>
+  <si>
+    <t>forma_pagamento</t>
+  </si>
+  <si>
+    <t>VARCHAR(45)</t>
+  </si>
+  <si>
+    <t>Forma de pagamento.</t>
+  </si>
+  <si>
     <t>id_usuario</t>
   </si>
   <si>
@@ -343,25 +361,48 @@
     <t>Id do orçamento ligado a venda.</t>
   </si>
   <si>
+    <t>Código de identificação
+ do orçamento.</t>
+  </si>
+  <si>
     <t>dataCriacao</t>
   </si>
   <si>
     <t>DATATIME</t>
   </si>
   <si>
+    <t>Data de criação do orçamento.</t>
+  </si>
+  <si>
     <t>dataValidade</t>
   </si>
   <si>
+    <t>Data de validade do orçamento.</t>
+  </si>
+  <si>
     <t>VARCHAR(20)</t>
   </si>
   <si>
+    <t>"pendente"</t>
+  </si>
+  <si>
+    <t>Status de venda do orçamento.</t>
+  </si>
+  <si>
     <t>informacoes</t>
   </si>
   <si>
     <t>TEXT</t>
   </si>
   <si>
+    <t>Informações adicionais que o ator 
+queira colocar no orçamento.</t>
+  </si>
+  <si>
     <t>id_cliente</t>
+  </si>
+  <si>
+    <t>Id do cliente ligado ao orçamento.</t>
   </si>
   <si>
     <t>Código de identificação
@@ -1216,7 +1257,7 @@
         <v>47</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>132</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4">
@@ -1234,7 +1275,7 @@
         <v>47</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>133</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5">
@@ -1252,16 +1293,16 @@
         <v>47</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>134</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" s="7"/>
       <c r="C6" s="3" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>79</v>
@@ -1270,13 +1311,13 @@
         <v>47</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>135</v>
+        <v>148</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="7"/>
       <c r="C7" s="2" t="s">
-        <v>136</v>
+        <v>149</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>50</v>
@@ -1288,13 +1329,13 @@
         <v>47</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>137</v>
+        <v>150</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" s="5"/>
       <c r="C8" s="3" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>45</v>
@@ -1306,7 +1347,7 @@
         <v>47</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>138</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -1375,13 +1416,13 @@
         <v>47</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>139</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" s="7"/>
       <c r="C4" s="3" t="s">
-        <v>140</v>
+        <v>153</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>45</v>
@@ -1399,7 +1440,7 @@
     <row r="5">
       <c r="B5" s="5"/>
       <c r="C5" s="2" t="s">
-        <v>141</v>
+        <v>154</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>45</v>
@@ -1480,13 +1521,13 @@
         <v>47</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>142</v>
+        <v>155</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" s="7"/>
       <c r="C4" s="3" t="s">
-        <v>143</v>
+        <v>156</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>45</v>
@@ -1498,13 +1539,13 @@
         <v>47</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>144</v>
+        <v>157</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" s="7"/>
       <c r="C5" s="2" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>45</v>
@@ -1516,7 +1557,7 @@
         <v>47</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>145</v>
+        <v>158</v>
       </c>
     </row>
     <row r="6">
@@ -1534,7 +1575,7 @@
         <v>47</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>146</v>
+        <v>159</v>
       </c>
     </row>
     <row r="7">
@@ -1552,16 +1593,16 @@
         <v>47</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>147</v>
+        <v>160</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" s="7"/>
       <c r="C8" s="9" t="s">
-        <v>148</v>
+        <v>161</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E8" s="9" t="s">
         <v>79</v>
@@ -1570,16 +1611,16 @@
         <v>47</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>149</v>
+        <v>162</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" s="5"/>
       <c r="C9" s="2" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>54</v>
@@ -1588,7 +1629,7 @@
         <v>47</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>151</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -2079,13 +2120,13 @@
         <v>47</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>58</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="5"/>
       <c r="C7" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>50</v>
@@ -2097,7 +2138,7 @@
         <v>47</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -2166,16 +2207,16 @@
         <v>47</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" s="7"/>
       <c r="C4" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>79</v>
@@ -2184,66 +2225,102 @@
         <v>47</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" s="7"/>
       <c r="C5" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>66</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>47</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" s="7"/>
-      <c r="C6" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="E6" s="3" t="s">
+      <c r="C6" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="F6" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="G6" s="3" t="s">
+      <c r="D6" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="F6" s="9">
+        <v>0.0</v>
+      </c>
+      <c r="G6" s="9" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="7">
-      <c r="B7" s="5"/>
+      <c r="B7" s="7"/>
       <c r="C7" s="2" t="s">
         <v>96</v>
       </c>
       <c r="D7" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" s="7"/>
+      <c r="C8" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>97</v>
+      <c r="E8" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" s="5"/>
+      <c r="C9" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B3:B7"/>
+    <mergeCell ref="B3:B9"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins bottom="1.0" footer="0.0" header="0.0" left="1.0" right="1.0" top="1.0"/>
@@ -2307,16 +2384,16 @@
         <v>47</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>48</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" s="7"/>
       <c r="C4" s="3" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>54</v>
@@ -2325,16 +2402,16 @@
         <v>47</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>51</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" s="7"/>
       <c r="C5" s="2" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>54</v>
@@ -2343,7 +2420,7 @@
         <v>47</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>55</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6">
@@ -2352,40 +2429,40 @@
         <v>71</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>54</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>47</v>
+        <v>111</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>58</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="7"/>
       <c r="C7" s="2" t="s">
-        <v>102</v>
+        <v>113</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>103</v>
+        <v>114</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>47</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>60</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" s="5"/>
       <c r="C8" s="3" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>45</v>
@@ -2397,7 +2474,7 @@
         <v>47</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>62</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -2466,7 +2543,7 @@
         <v>47</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>105</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4">
@@ -2484,7 +2561,7 @@
         <v>47</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>106</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5">
@@ -2502,16 +2579,16 @@
         <v>47</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>107</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" s="7"/>
       <c r="C6" s="3" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>109</v>
+        <v>122</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>79</v>
@@ -2520,13 +2597,13 @@
         <v>47</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="7"/>
       <c r="C7" s="2" t="s">
-        <v>111</v>
+        <v>124</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>50</v>
@@ -2538,7 +2615,7 @@
         <v>47</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>112</v>
+        <v>125</v>
       </c>
     </row>
     <row r="8">
@@ -2556,13 +2633,13 @@
         <v>47</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>113</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" s="7"/>
       <c r="C9" s="2" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>53</v>
@@ -2574,13 +2651,13 @@
         <v>47</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>115</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" s="7"/>
       <c r="C10" s="3" t="s">
-        <v>116</v>
+        <v>129</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>45</v>
@@ -2592,7 +2669,7 @@
         <v>47</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>117</v>
+        <v>130</v>
       </c>
     </row>
     <row r="11">
@@ -2610,7 +2687,7 @@
         <v>1.0</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>118</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -2679,7 +2756,7 @@
         <v>47</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>119</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4">
@@ -2688,7 +2765,7 @@
         <v>52</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>120</v>
+        <v>133</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>54</v>
@@ -2697,13 +2774,13 @@
         <v>47</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>121</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" s="7"/>
       <c r="C5" s="2" t="s">
-        <v>122</v>
+        <v>135</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>50</v>
@@ -2715,7 +2792,7 @@
         <v>47</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>123</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6">
@@ -2733,7 +2810,7 @@
         <v>47</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>124</v>
+        <v>137</v>
       </c>
     </row>
     <row r="7">
@@ -2751,7 +2828,7 @@
         <v>1.0</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>125</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -2820,7 +2897,7 @@
         <v>47</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>126</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4">
@@ -2829,7 +2906,7 @@
         <v>52</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>120</v>
+        <v>133</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>79</v>
@@ -2838,7 +2915,7 @@
         <v>47</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>127</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5">
@@ -2856,13 +2933,13 @@
         <v>47</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>128</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" s="7"/>
       <c r="C6" s="3" t="s">
-        <v>129</v>
+        <v>142</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>72</v>
@@ -2874,7 +2951,7 @@
         <v>47</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>130</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7">
@@ -2892,7 +2969,7 @@
         <v>1.0</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>131</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>